<commit_message>
Changes made in DD & rentalincome_dw added
</commit_message>
<xml_diff>
--- a/docs/DataAnalysis.xlsx
+++ b/docs/DataAnalysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulnur.dogotari/Desktop/CIS4400/HW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gulnur.dogotari/Desktop/CIS4400/HW/code/rentalincome/rental_income_nyc/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C780451B-0646-E649-8171-13092A7A9C4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F8951A-12A4-2B4B-A188-E52FE87263B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7840" yWindow="500" windowWidth="20960" windowHeight="16460" xr2:uid="{3BD4163E-51DA-5143-88CF-448D0C4956C3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16780" windowHeight="16460" xr2:uid="{3BD4163E-51DA-5143-88CF-448D0C4956C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
   <si>
     <t>Data Engineering</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>Dim_Location</t>
-  </si>
-  <si>
-    <t>Street_Number</t>
   </si>
   <si>
     <t>Street</t>
@@ -615,7 +612,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -720,16 +717,13 @@
       <c r="E12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="L12" s="7" t="s">
+      <c r="L12" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>